<commit_message>
v3.4 With tampered eval
Tampered evaluation give slightly better scores over 1000 games.
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://templestowecvicedu-my.sharepoint.com/personal/ric0016_tc_vic_edu_au/Documents/Desktop/Documents/GitHub/Rohan_Chess_Bot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://templestowecvicedu-my.sharepoint.com/personal/ric0016_tc_vic_edu_au/Documents/Desktop/Coding/Rohan_Chess_Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{5F099AA7-ECCD-4D90-8E93-F6F22C21EE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7927F6AF-BA0E-46BF-9AE4-102688C6F9CC}"/>
+  <xr:revisionPtr revIDLastSave="366" documentId="13_ncr:1_{5F099AA7-ECCD-4D90-8E93-F6F22C21EE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E5DBDFA-9D58-44F1-956F-5F359E382D85}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="21164" windowHeight="11291" xr2:uid="{F2D52949-C3DC-4F2A-841B-DD6F0E0EB30B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="287">
   <si>
     <t>1.6.2</t>
   </si>
@@ -774,6 +774,184 @@
   <si>
     <t>2.8b</t>
   </si>
+  <si>
+    <t>2.8c</t>
+  </si>
+  <si>
+    <t>2.8d</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>MyBot (New, Fixed SEE)</t>
+  </si>
+  <si>
+    <t>EvilBot (Old, Buggy SEE)</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>Data Points Analyzed</t>
+  </si>
+  <si>
+    <t>Average Depth</t>
+  </si>
+  <si>
+    <t>Average Nodes / Move</t>
+  </si>
+  <si>
+    <t>Average NPS</t>
+  </si>
+  <si>
+    <t>Nodes per Ply of Depth</t>
+  </si>
+  <si>
+    <r>
+      <t>Quantitative Analysis: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>MyBot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (Fixed) vs. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>EvilBot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (Buggy)</t>
+    </r>
+  </si>
+  <si>
+    <t>2.8e</t>
+  </si>
+  <si>
+    <t>2.9a</t>
+  </si>
+  <si>
+    <t>2.9b</t>
+  </si>
+  <si>
+    <t>2.9c</t>
+  </si>
+  <si>
+    <t>2.9d</t>
+  </si>
+  <si>
+    <t>800 games</t>
+  </si>
+  <si>
+    <t>2.9 final</t>
+  </si>
+  <si>
+    <t>9s + 55ms:</t>
+  </si>
+  <si>
+    <t>2.9.1</t>
+  </si>
+  <si>
+    <t>2.9.2</t>
+  </si>
+  <si>
+    <t>2.9.3</t>
+  </si>
+  <si>
+    <t>2.9.4</t>
+  </si>
+  <si>
+    <t>250g 3+25ms showdown</t>
+  </si>
+  <si>
+    <t>5s_32ms</t>
+  </si>
+  <si>
+    <t>3.1b</t>
+  </si>
+  <si>
+    <t>3.1.1</t>
+  </si>
+  <si>
+    <t>3.2b</t>
+  </si>
+  <si>
+    <t>3.3e futil safe promotions</t>
+  </si>
+  <si>
+    <t>v3.3 Final (PLUG)</t>
+  </si>
+  <si>
+    <t>v3.3 Final (UNPLUG)</t>
+  </si>
+  <si>
+    <t>5s 32ms</t>
+  </si>
+  <si>
+    <t>3.3d</t>
+  </si>
+  <si>
+    <t>v3.3 (10s 64ms plug)</t>
+  </si>
+  <si>
+    <t>3.3.1 (unplug 7_40)</t>
+  </si>
+  <si>
+    <t>v3.4a (6_35 unp)</t>
+  </si>
+  <si>
+    <t>v3.4a (5_35 plug)</t>
+  </si>
+  <si>
+    <t>3.4a (10_70 plug)</t>
+  </si>
+  <si>
+    <t>3.3f</t>
+  </si>
+  <si>
+    <t>3.3g</t>
+  </si>
+  <si>
+    <t>5_35</t>
+  </si>
+  <si>
+    <t>3.3h</t>
+  </si>
+  <si>
+    <t>3.3i</t>
+  </si>
+  <si>
+    <t>3.3j</t>
+  </si>
+  <si>
+    <t>3.3k</t>
+  </si>
+  <si>
+    <t>3.3k plug</t>
+  </si>
+  <si>
+    <t>3.3.1</t>
+  </si>
 </sst>
 </file>
 
@@ -783,7 +961,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -817,6 +995,42 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFE2E2E5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFE2E2E5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FFE2E2E5"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -839,7 +1053,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -861,6 +1075,49 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1308,10 +1565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D4B1D1-FAE6-4108-A8C2-E7557A93D445}">
-  <dimension ref="A1:I329"/>
+  <dimension ref="A1:I393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A308" workbookViewId="0">
-      <selection activeCell="D320" sqref="D320"/>
+    <sheetView tabSelected="1" topLeftCell="A379" zoomScale="84" workbookViewId="0">
+      <selection activeCell="E394" sqref="E394"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.2" x14ac:dyDescent="0.3"/>
@@ -1320,14 +1577,14 @@
     <col min="2" max="2" width="35.09765625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.296875" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.8984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="39.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.796875" style="1"/>
-    <col min="8" max="8" width="38.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.19921875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.3984375" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="14.35" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1335,7 +1592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="14.35" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1343,7 +1600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="14.35" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1351,7 +1608,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="4" spans="2:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" s="2" customFormat="1" ht="14.35" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1363,12 +1620,12 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="14.35" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="14.35" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>1.8</v>
       </c>
@@ -1381,7 +1638,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="14.35" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1397,7 +1654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="14.35" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1411,7 +1668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" ht="14.35" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1422,7 +1679,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" ht="14.35" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1433,12 +1690,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" ht="14.35" x14ac:dyDescent="0.3">
       <c r="C16" s="1">
         <v>1.8</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="14.35" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
@@ -1446,7 +1703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="14.35" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
@@ -1472,7 +1729,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="14.35" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1500,7 +1757,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="14.35" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
@@ -1511,7 +1768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="14.35" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -1526,7 +1783,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="14.35" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -1537,7 +1794,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="14.35" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
@@ -1552,7 +1809,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="14.35" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -1567,7 +1824,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="14.35" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -1581,7 +1838,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="14.35" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
@@ -1592,7 +1849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="14.35" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -1603,7 +1860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="14.35" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>28</v>
       </c>
@@ -1611,7 +1868,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="14.35" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>30</v>
       </c>
@@ -1623,7 +1880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="14.35" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
@@ -1635,7 +1892,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="14.35" x14ac:dyDescent="0.3">
       <c r="C37" s="1" t="s">
         <v>21</v>
       </c>
@@ -1643,7 +1900,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="14.35" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>31</v>
       </c>
@@ -1658,7 +1915,7 @@
         <v>-18</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="14.35" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>32</v>
       </c>
@@ -1666,7 +1923,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="14.35" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>14</v>
       </c>
@@ -1675,12 +1932,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="14.35" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="14.35" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>34</v>
       </c>
@@ -1697,7 +1954,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>33</v>
       </c>
@@ -1717,7 +1974,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B48" s="1" t="s">
         <v>37</v>
       </c>
@@ -1725,7 +1982,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>36</v>
       </c>
@@ -1737,12 +1994,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C51" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>39</v>
       </c>
@@ -1753,7 +2010,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>41</v>
       </c>
@@ -1764,7 +2021,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>34</v>
       </c>
@@ -1784,12 +2041,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B57" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>5</v>
       </c>
@@ -1800,7 +2057,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>44</v>
       </c>
@@ -1812,7 +2069,7 @@
         <v>-24</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>46</v>
       </c>
@@ -1824,7 +2081,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>47</v>
       </c>
@@ -1839,7 +2096,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>57</v>
       </c>
@@ -1851,12 +2108,12 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B65" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>50</v>
       </c>
@@ -1865,7 +2122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>51</v>
       </c>
@@ -1874,12 +2131,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B69" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>52</v>
       </c>
@@ -1888,12 +2145,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>56</v>
       </c>
@@ -1902,7 +2159,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>15</v>
       </c>
@@ -1910,7 +2167,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>58</v>
       </c>
@@ -1919,12 +2176,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B77" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>59</v>
       </c>
@@ -1933,7 +2190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>60</v>
       </c>
@@ -1942,7 +2199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>61</v>
       </c>
@@ -1953,7 +2210,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>63</v>
       </c>
@@ -1964,7 +2221,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>64</v>
       </c>
@@ -1973,12 +2230,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B84" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>65</v>
       </c>
@@ -1986,7 +2243,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>13</v>
       </c>
@@ -1994,7 +2251,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>66</v>
       </c>
@@ -2003,12 +2260,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B90" s="1">
         <v>2.1</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>68</v>
       </c>
@@ -2016,7 +2273,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -2024,7 +2281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>37</v>
       </c>
@@ -2032,7 +2289,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>69</v>
       </c>
@@ -2041,7 +2298,7 @@
         <v>-38</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>70</v>
       </c>
@@ -2050,7 +2307,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>71</v>
       </c>
@@ -2058,7 +2315,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>72</v>
       </c>
@@ -2067,7 +2324,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>75</v>
       </c>
@@ -2078,7 +2335,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>73</v>
       </c>
@@ -2091,7 +2348,7 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>76</v>
       </c>
@@ -2107,7 +2364,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>80</v>
       </c>
@@ -2138,12 +2395,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B108" s="1">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>84</v>
       </c>
@@ -2152,7 +2409,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>85</v>
       </c>
@@ -2161,7 +2418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>86</v>
       </c>
@@ -2170,7 +2427,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>87</v>
       </c>
@@ -2179,7 +2436,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>88</v>
       </c>
@@ -2187,12 +2444,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B116" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>2.5</v>
       </c>
@@ -2201,12 +2458,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B118" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>89</v>
       </c>
@@ -2215,12 +2472,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B121" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>90</v>
       </c>
@@ -2229,7 +2486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>13</v>
       </c>
@@ -2237,7 +2494,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>92</v>
       </c>
@@ -2246,7 +2503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B128" s="1" t="s">
         <v>93</v>
       </c>
@@ -2260,7 +2517,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B129" s="1" t="s">
         <v>91</v>
       </c>
@@ -2273,12 +2530,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B132" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B133" s="1" t="s">
         <v>94</v>
       </c>
@@ -2286,7 +2543,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B134" s="1">
         <v>0.2</v>
       </c>
@@ -2298,7 +2555,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B135" s="1" t="s">
         <v>96</v>
       </c>
@@ -2307,7 +2564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B136" s="1" t="s">
         <v>97</v>
       </c>
@@ -2316,7 +2573,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B138" s="1" t="s">
         <v>98</v>
       </c>
@@ -2324,7 +2581,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B139" s="1">
         <v>0.4</v>
       </c>
@@ -2335,7 +2592,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B140" s="1" t="s">
         <v>101</v>
       </c>
@@ -2347,7 +2604,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B141" s="1">
         <v>0.5</v>
       </c>
@@ -2356,7 +2613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B143" s="1" t="s">
         <v>103</v>
       </c>
@@ -2364,7 +2621,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B144" s="1">
         <v>0.6</v>
       </c>
@@ -2373,7 +2630,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B145" s="1">
         <v>0.7</v>
       </c>
@@ -2385,7 +2642,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B146" s="1" t="s">
         <v>105</v>
       </c>
@@ -2394,7 +2651,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B149" s="1" t="s">
         <v>106</v>
       </c>
@@ -2402,7 +2659,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B150" s="1" t="s">
         <v>110</v>
       </c>
@@ -2411,12 +2668,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B152" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B153" s="1" t="s">
         <v>107</v>
       </c>
@@ -2424,7 +2681,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B154" s="1" t="s">
         <v>109</v>
       </c>
@@ -2436,7 +2693,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B155" s="1" t="s">
         <v>111</v>
       </c>
@@ -2448,7 +2705,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B156" s="1" t="s">
         <v>113</v>
       </c>
@@ -2457,7 +2714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B157" s="1" t="s">
         <v>114</v>
       </c>
@@ -2469,7 +2726,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B160" s="1" t="s">
         <v>106</v>
       </c>
@@ -2477,7 +2734,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="161" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B161" s="1">
         <v>1.2</v>
       </c>
@@ -2489,7 +2746,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B162" s="1">
         <v>1.3</v>
       </c>
@@ -2501,7 +2758,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="163" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B163" s="1" t="s">
         <v>119</v>
       </c>
@@ -2513,7 +2770,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B164" s="1">
         <v>1.4</v>
       </c>
@@ -2525,7 +2782,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B166" s="1" t="s">
         <v>13</v>
       </c>
@@ -2533,7 +2790,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="167" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B167" s="1" t="s">
         <v>122</v>
       </c>
@@ -2545,7 +2802,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="168" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B168" s="1" t="s">
         <v>123</v>
       </c>
@@ -2554,7 +2811,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="169" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B169" s="1" t="s">
         <v>124</v>
       </c>
@@ -2563,7 +2820,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="170" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B170" s="1">
         <v>1.6</v>
       </c>
@@ -2575,7 +2832,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="171" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B171" s="1">
         <v>1.7</v>
       </c>
@@ -2587,7 +2844,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="174" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B174" s="1" t="s">
         <v>127</v>
       </c>
@@ -2604,7 +2861,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="175" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B175" s="1">
         <v>1.7</v>
       </c>
@@ -2625,12 +2882,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="176" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B176" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="179" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B179" s="1">
         <v>1000</v>
       </c>
@@ -2647,7 +2904,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="180" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B180" s="1">
         <v>1.7</v>
       </c>
@@ -2667,12 +2924,12 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="182" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C182" s="1">
         <v>1.7</v>
       </c>
     </row>
-    <row r="183" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B183" s="1" t="s">
         <v>135</v>
       </c>
@@ -2681,7 +2938,7 @@
         <v>-23</v>
       </c>
     </row>
-    <row r="184" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B184" s="1" t="s">
         <v>136</v>
       </c>
@@ -2697,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B186" s="1" t="s">
         <v>138</v>
       </c>
@@ -2705,7 +2962,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="187" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B187" s="1" t="s">
         <v>139</v>
       </c>
@@ -2713,7 +2970,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="188" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B188" s="1" t="s">
         <v>140</v>
       </c>
@@ -2721,7 +2978,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="189" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B189" s="1" t="s">
         <v>141</v>
       </c>
@@ -2730,12 +2987,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="190" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B190" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="191" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B191" s="1" t="s">
         <v>142</v>
       </c>
@@ -2744,7 +3001,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="192" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B192" s="1" t="s">
         <v>143</v>
       </c>
@@ -2753,7 +3010,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B193" s="1" t="s">
         <v>144</v>
       </c>
@@ -2764,7 +3021,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B194" s="1" t="s">
         <v>146</v>
       </c>
@@ -2775,7 +3032,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B195" s="1" t="s">
         <v>148</v>
       </c>
@@ -2783,7 +3040,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B196" s="1" t="s">
         <v>15</v>
       </c>
@@ -2800,7 +3057,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B197" s="1" t="s">
         <v>149</v>
       </c>
@@ -2820,12 +3077,12 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C200" s="1">
         <v>1.7</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B201" s="1" t="s">
         <v>152</v>
       </c>
@@ -2834,7 +3091,7 @@
         <v>-22</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B202" s="1" t="s">
         <v>153</v>
       </c>
@@ -2843,7 +3100,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B203" s="1" t="s">
         <v>154</v>
       </c>
@@ -2852,7 +3109,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B205" s="1" t="s">
         <v>155</v>
       </c>
@@ -2861,7 +3118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>157</v>
       </c>
@@ -2873,7 +3130,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B207" s="1" t="s">
         <v>158</v>
       </c>
@@ -2882,7 +3139,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B208" s="1" t="s">
         <v>159</v>
       </c>
@@ -2891,12 +3148,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="210" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C210" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="211" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B211" s="1" t="s">
         <v>161</v>
       </c>
@@ -2905,12 +3162,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C213" s="1">
         <v>1.8</v>
       </c>
     </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B214" s="1" t="s">
         <v>162</v>
       </c>
@@ -2918,7 +3175,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="215" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B215" s="1" t="s">
         <v>163</v>
       </c>
@@ -2926,7 +3183,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="216" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B216" s="1" t="s">
         <v>164</v>
       </c>
@@ -2934,7 +3191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B217" s="1" t="s">
         <v>165</v>
       </c>
@@ -2943,12 +3200,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="219" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C219" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="220" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B220" s="1" t="s">
         <v>166</v>
       </c>
@@ -2957,7 +3214,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="222" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B222" s="1" t="s">
         <v>168</v>
       </c>
@@ -2965,7 +3222,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="223" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B223" s="1" t="s">
         <v>167</v>
       </c>
@@ -2973,7 +3230,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="224" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B224" s="1" t="s">
         <v>169</v>
       </c>
@@ -2982,7 +3239,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="225" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B225" s="1" t="s">
         <v>170</v>
       </c>
@@ -2991,12 +3248,12 @@
         <v>24.714285714285715</v>
       </c>
     </row>
-    <row r="227" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="227" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C227" s="1">
         <v>1.9</v>
       </c>
     </row>
-    <row r="228" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="228" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B228" s="1" t="s">
         <v>172</v>
       </c>
@@ -3005,7 +3262,7 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="229" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="229" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B229" s="1" t="s">
         <v>171</v>
       </c>
@@ -3013,7 +3270,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="230" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="230" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B230" s="1" t="s">
         <v>173</v>
       </c>
@@ -3021,7 +3278,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="231" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="231" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B231" s="1" t="s">
         <v>174</v>
       </c>
@@ -3029,7 +3286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="232" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B232" s="1" t="s">
         <v>175</v>
       </c>
@@ -3038,7 +3295,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="233" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="233" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B233" s="1" t="s">
         <v>176</v>
       </c>
@@ -3046,7 +3303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="234" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B234" s="1" t="s">
         <v>177</v>
       </c>
@@ -3055,7 +3312,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="235" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="235" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B235" s="1" t="s">
         <v>178</v>
       </c>
@@ -3064,7 +3321,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="236" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="236" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B236" s="1" t="s">
         <v>179</v>
       </c>
@@ -3072,12 +3329,12 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="238" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="238" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C238" s="1">
         <v>1.9</v>
       </c>
     </row>
-    <row r="239" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="239" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B239" s="1" t="s">
         <v>180</v>
       </c>
@@ -3086,12 +3343,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="241" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="241" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C241" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="242" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="242" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B242" s="1" t="s">
         <v>45</v>
       </c>
@@ -3100,7 +3357,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="245" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="245" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B245" s="1" t="s">
         <v>181</v>
       </c>
@@ -3120,7 +3377,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="246" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="246" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B246" s="1" t="s">
         <v>45</v>
       </c>
@@ -3145,12 +3402,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="248" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="248" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C248" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="249" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="249" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B249" s="1" t="s">
         <v>48</v>
       </c>
@@ -3159,12 +3416,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="251" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="251" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C251" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="252" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="252" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B252" s="1" t="s">
         <v>184</v>
       </c>
@@ -3172,7 +3429,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="253" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="253" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B253" s="1" t="s">
         <v>187</v>
       </c>
@@ -3180,7 +3437,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="255" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="255" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B255" s="1">
         <v>2.1</v>
       </c>
@@ -3188,7 +3445,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="257" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="257" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B257" s="1" t="s">
         <v>189</v>
       </c>
@@ -3199,7 +3456,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="258" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="258" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B258" s="1" t="s">
         <v>188</v>
       </c>
@@ -3211,7 +3468,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="259" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="259" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B259" s="1" t="s">
         <v>190</v>
       </c>
@@ -3223,7 +3480,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="260" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="260" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B260" s="1" t="s">
         <v>191</v>
       </c>
@@ -3235,7 +3492,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="261" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="261" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B261" s="1" t="s">
         <v>195</v>
       </c>
@@ -3244,7 +3501,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="262" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="262" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B262" s="1" t="s">
         <v>196</v>
       </c>
@@ -3253,12 +3510,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="264" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="264" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C264" s="1">
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="265" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="265" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B265" s="1" t="s">
         <v>197</v>
       </c>
@@ -3269,7 +3526,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="266" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="266" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B266" s="1" t="s">
         <v>198</v>
       </c>
@@ -3280,7 +3537,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="267" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="267" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B267" s="1" t="s">
         <v>199</v>
       </c>
@@ -3292,7 +3549,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="268" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="268" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B268" s="1" t="s">
         <v>200</v>
       </c>
@@ -3304,7 +3561,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="269" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="269" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B269" s="1" t="s">
         <v>201</v>
       </c>
@@ -3316,7 +3573,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="270" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="270" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B270" s="1" t="s">
         <v>202</v>
       </c>
@@ -3328,7 +3585,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="273" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="273" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C273" s="1">
         <v>2.2999999999999998</v>
       </c>
@@ -3351,12 +3608,12 @@
         <v>205</v>
       </c>
     </row>
-    <row r="276" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="276" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C276" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="277" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="277" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B277" s="1" t="s">
         <v>207</v>
       </c>
@@ -3364,7 +3621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="278" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B278" s="1" t="s">
         <v>208</v>
       </c>
@@ -3376,12 +3633,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="280" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="280" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C280" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="281" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="281" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B281" s="1" t="s">
         <v>209</v>
       </c>
@@ -3390,7 +3647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="282" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B282" s="1" t="s">
         <v>211</v>
       </c>
@@ -3399,7 +3656,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="284" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="284" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B284" s="1" t="s">
         <v>212</v>
       </c>
@@ -3416,7 +3673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="285" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="285" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B285" s="1">
         <v>2.4</v>
       </c>
@@ -3436,7 +3693,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="287" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="287" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B287" s="1" t="s">
         <v>214</v>
       </c>
@@ -3444,7 +3701,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="288" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="288" spans="2:6" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B288" s="1" t="s">
         <v>213</v>
       </c>
@@ -3453,7 +3710,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="289" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="289" spans="2:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B289" s="1" t="s">
         <v>215</v>
       </c>
@@ -3462,7 +3719,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="290" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="290" spans="2:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B290" s="1" t="s">
         <v>216</v>
       </c>
@@ -3471,12 +3728,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="292" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="292" spans="2:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C292" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="293" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="293" spans="2:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B293" s="1" t="s">
         <v>217</v>
       </c>
@@ -3484,12 +3741,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="295" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="295" spans="2:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C295" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="296" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="296" spans="2:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B296" s="1" t="s">
         <v>218</v>
       </c>
@@ -3497,17 +3754,17 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="297" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="297" spans="2:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B297" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="298" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="298" spans="2:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C298" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="299" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="299" spans="2:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B299" s="1" t="s">
         <v>220</v>
       </c>
@@ -3516,7 +3773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="300" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="300" spans="2:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B300" s="1" t="s">
         <v>221</v>
       </c>
@@ -3525,7 +3782,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="301" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="301" spans="2:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B301" s="1" t="s">
         <v>222</v>
       </c>
@@ -3534,7 +3791,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="303" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="303" spans="2:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B303" s="1" t="s">
         <v>225</v>
       </c>
@@ -3548,7 +3805,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="304" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="304" spans="2:5" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B304" s="1">
         <v>2.5</v>
       </c>
@@ -3565,7 +3822,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="306" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="306" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B306" s="1" t="s">
         <v>227</v>
       </c>
@@ -3573,7 +3830,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="307" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="307" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B307" s="1" t="s">
         <v>228</v>
       </c>
@@ -3581,7 +3838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="308" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B308" s="1" t="s">
         <v>229</v>
       </c>
@@ -3589,12 +3846,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="310" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="310" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C310" s="1">
         <v>2.6</v>
       </c>
     </row>
-    <row r="311" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="311" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B311" s="1" t="s">
         <v>230</v>
       </c>
@@ -3602,7 +3859,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="313" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="313" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B313" s="1" t="s">
         <v>13</v>
       </c>
@@ -3610,7 +3867,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="314" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="314" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B314" s="1">
         <v>2.7</v>
       </c>
@@ -3619,12 +3876,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="316" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="316" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C316" s="1">
         <v>2.7</v>
       </c>
     </row>
-    <row r="317" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="317" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B317" s="1" t="s">
         <v>231</v>
       </c>
@@ -3632,18 +3889,18 @@
         <v>232</v>
       </c>
     </row>
-    <row r="318" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="318" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C318" s="1">
         <f>20-46</f>
         <v>-26</v>
       </c>
     </row>
-    <row r="320" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="320" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C320" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="321" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="321" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B321" s="1" t="s">
         <v>233</v>
       </c>
@@ -3651,7 +3908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="322" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B322" s="1" t="s">
         <v>234</v>
       </c>
@@ -3660,7 +3917,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="324" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="324" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B324" s="1" t="s">
         <v>13</v>
       </c>
@@ -3671,7 +3928,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="325" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="325" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B325" s="1" t="s">
         <v>236</v>
       </c>
@@ -3684,7 +3941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="326" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="326" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B326" s="1" t="s">
         <v>237</v>
       </c>
@@ -3697,15 +3954,15 @@
         <v>-13</v>
       </c>
     </row>
-    <row r="327" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="327" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B327" s="7"/>
     </row>
-    <row r="328" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="328" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
       <c r="C328" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="329" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="329" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
       <c r="B329" s="1" t="s">
         <v>238</v>
       </c>
@@ -3714,7 +3971,554 @@
         <v>-26</v>
       </c>
     </row>
+    <row r="330" spans="2:8" ht="15.3" x14ac:dyDescent="0.3">
+      <c r="B330" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C330" s="1">
+        <v>3</v>
+      </c>
+      <c r="E330" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="F330" s="22"/>
+      <c r="G330" s="8"/>
+      <c r="H330" s="8"/>
+    </row>
+    <row r="331" spans="2:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B331" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C331" s="1">
+        <f>131-113</f>
+        <v>18</v>
+      </c>
+      <c r="E331" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="F331" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="G331" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="H331" s="9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="332" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="E332" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="F332" s="10">
+        <v>204</v>
+      </c>
+      <c r="G332" s="10">
+        <v>205</v>
+      </c>
+      <c r="H332" s="10"/>
+    </row>
+    <row r="333" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="C333" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E333" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="F333" s="9">
+        <v>5.47</v>
+      </c>
+      <c r="G333" s="10">
+        <v>5.09</v>
+      </c>
+      <c r="H333" s="11">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="334" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B334" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C334" s="1">
+        <f>94-103</f>
+        <v>-9</v>
+      </c>
+      <c r="E334" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="F334" s="12">
+        <v>13874</v>
+      </c>
+      <c r="G334" s="12">
+        <v>14039</v>
+      </c>
+      <c r="H334" s="13">
+        <v>-1.2E-2</v>
+      </c>
+    </row>
+    <row r="335" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B335" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C335" s="1">
+        <f>92-74</f>
+        <v>18</v>
+      </c>
+      <c r="E335" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="F335" s="12">
+        <v>185559</v>
+      </c>
+      <c r="G335" s="14">
+        <v>192206</v>
+      </c>
+      <c r="H335" s="13">
+        <v>-3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="336" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="E336" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="F336" s="12">
+        <v>2536</v>
+      </c>
+      <c r="G336" s="12">
+        <v>2758</v>
+      </c>
+      <c r="H336" s="11">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="337" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B337" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="338" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B338" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C338" s="1">
+        <v>-5</v>
+      </c>
+      <c r="E338" s="15"/>
+      <c r="F338" s="16"/>
+      <c r="G338" s="16"/>
+      <c r="H338" s="15"/>
+    </row>
+    <row r="339" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B339" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C339" s="1">
+        <f>103-84</f>
+        <v>19</v>
+      </c>
+      <c r="E339" s="15"/>
+      <c r="F339" s="17"/>
+      <c r="G339" s="17"/>
+      <c r="H339" s="17"/>
+    </row>
+    <row r="340" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="E340" s="15"/>
+      <c r="F340" s="17"/>
+      <c r="G340" s="17"/>
+      <c r="H340" s="18"/>
+    </row>
+    <row r="341" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="C341" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E341" s="15"/>
+      <c r="F341" s="19"/>
+      <c r="G341" s="19"/>
+      <c r="H341" s="20"/>
+    </row>
+    <row r="342" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B342" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C342" s="1">
+        <f>150-151</f>
+        <v>-1</v>
+      </c>
+      <c r="E342" s="15"/>
+      <c r="F342" s="19"/>
+      <c r="G342" s="21"/>
+      <c r="H342" s="20"/>
+    </row>
+    <row r="343" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="E343" s="15"/>
+      <c r="F343" s="19"/>
+      <c r="G343" s="19"/>
+      <c r="H343" s="18"/>
+    </row>
+    <row r="344" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B344" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C344" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="D344" s="1">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="345" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B345" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="C345" s="1">
+        <f>325-380</f>
+        <v>-55</v>
+      </c>
+      <c r="D345" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="346" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B346" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C346" s="1">
+        <f>290-295</f>
+        <v>-5</v>
+      </c>
+      <c r="D346" s="1">
+        <f>180-171</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="347" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B347" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C347" s="1">
+        <f>128-117</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="348" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B348" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C348" s="1">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="349" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B349" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C349" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="350" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B350" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C350" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="351" spans="2:8" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B351" s="1">
+        <v>3</v>
+      </c>
+      <c r="C351" s="1">
+        <f>169-148</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="353" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B353" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C353" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="D353" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="E353" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="F353" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="G353" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="354" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B354" s="1">
+        <v>3</v>
+      </c>
+      <c r="C354" s="1">
+        <f>(355-385)/3</f>
+        <v>-10</v>
+      </c>
+      <c r="D354" s="1">
+        <f>300-300</f>
+        <v>0</v>
+      </c>
+      <c r="E354" s="1">
+        <f>100-103</f>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="358" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B358" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C358" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="359" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B359" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="C359" s="1">
+        <f>140-202</f>
+        <v>-62</v>
+      </c>
+    </row>
+    <row r="360" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B360" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C360" s="1">
+        <f>148-93</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="363" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="C363" s="1">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="364" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B364" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C364" s="1">
+        <f>47-46</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="366" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="C366" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="367" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B367" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="C367" s="1">
+        <f>80-113</f>
+        <v>-33</v>
+      </c>
+    </row>
+    <row r="368" spans="2:7" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B368" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C368" s="1">
+        <f>448-404</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="371" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B371" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C371" s="1">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="372" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B372" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C372" s="1">
+        <f>142-158</f>
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="373" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B373" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C373" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B374" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C374" s="1">
+        <f>69-104</f>
+        <v>-35</v>
+      </c>
+      <c r="D374" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="375" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B375" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C375" s="1">
+        <f>155-159</f>
+        <v>-4</v>
+      </c>
+      <c r="D375" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="376" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B376" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C376" s="1">
+        <f>61-65</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="378" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B378" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C378" s="1">
+        <f>73-82</f>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="379" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B379" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C379" s="1">
+        <f>46-75</f>
+        <v>-29</v>
+      </c>
+    </row>
+    <row r="380" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B380" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C380" s="1">
+        <f>91-107</f>
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="381" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B381" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C381" s="1">
+        <f>49-75</f>
+        <v>-26</v>
+      </c>
+    </row>
+    <row r="383" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B383" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C383" s="1">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="384" spans="2:4" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B384" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C384" s="1">
+        <v>-10000</v>
+      </c>
+    </row>
+    <row r="385" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B385" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C385" s="1">
+        <f>152-147</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="386" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B386" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C386" s="1">
+        <f>227-314</f>
+        <v>-87</v>
+      </c>
+    </row>
+    <row r="387" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B387" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C387" s="1">
+        <f>59-78</f>
+        <v>-19</v>
+      </c>
+    </row>
+    <row r="388" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B388" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C388" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B389" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C389" s="1">
+        <f>44-44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="390" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B390" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C390" s="1">
+        <f>77-56</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="392" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="C392" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="393" spans="2:3" ht="14.05" x14ac:dyDescent="0.3">
+      <c r="B393" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="C393" s="1">
+        <f>470-358</f>
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E330:F330"/>
+  </mergeCells>
   <conditionalFormatting sqref="C139">
     <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>0</formula>

</xml_diff>